<commit_message>
#22 fixed errors on axes for statement of activities; still need to fix domain validation errors
</commit_message>
<xml_diff>
--- a/static/input_files/samples/Clayton.xlsx
+++ b/static/input_files/samples/Clayton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C92D96-0408-804B-AF46-9190415943FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A179509-6504-9544-B457-F44DF4903459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34700" yWindow="-8560" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -22224,8 +22224,8 @@
   </sheetPr>
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -24166,8 +24166,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>